<commit_message>
Q 9 corrected, Q 15 corrected
</commit_message>
<xml_diff>
--- a/globallogic_mcqtest.xlsx
+++ b/globallogic_mcqtest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="208">
   <si>
     <t xml:space="preserve">   </t>
   </si>
@@ -223,6 +223,30 @@
     <t xml:space="preserve">D)none of the above</t>
   </si>
   <si>
+    <t xml:space="preserve">String k ="big ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k.concat("crowded ");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k += "city";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System.out.println(k);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a) big crowded city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b) big city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c) big crowded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d) Compile error</t>
+  </si>
+  <si>
     <t xml:space="preserve">What will you do if you don’t want to handle a checked CustomException occuing in method?</t>
   </si>
   <si>
@@ -289,7 +313,16 @@
     <t xml:space="preserve">All of the above</t>
   </si>
   <si>
-    <t xml:space="preserve">Which implementation of set will you use to keep elements in sorted order?</t>
+    <t xml:space="preserve">Which implementation of Map will you use to keep elements in insertion order?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HashMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedHashMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreeMap</t>
   </si>
   <si>
     <t xml:space="preserve">    class Code</t>
@@ -310,51 +343,54 @@
     <t xml:space="preserve">           {</t>
   </si>
   <si>
+    <t xml:space="preserve">               int a=0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               int num= 5;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               int result = num / a;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               System.out.print("Good");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           }</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> catch(ArithmeticException e) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               System.out.print("Evening");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           catch(Exception e) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               System.out.print("Morning");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoodEveningMorning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoodMorning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compilation Failure</t>
+  </si>
+  <si>
     <t xml:space="preserve">               Int a=0;</t>
   </si>
   <si>
-    <t xml:space="preserve">               int num= 5;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               int result = num / a;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               System.out.print("Good");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           }</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> catch(ArithmeticException e) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">               System.out.print("Evening");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">           catch(Exception e) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">               System.out.print("Morning");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GoodEveningMorning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GoodMorning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compilation Failure</t>
-  </si>
-  <si>
     <t xml:space="preserve"> catch(Exception e) </t>
   </si>
   <si>
@@ -461,30 +497,6 @@
   </si>
   <si>
     <t xml:space="preserve">d) Compile Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String k ="big ";</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k.concat("crowded ");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k += "city";</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System.out.println(k);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a) big crowded city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b) big city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c) big crowded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d) Compile error</t>
   </si>
   <si>
     <t xml:space="preserve">The following code:</t>
@@ -695,12 +707,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Times New Roman"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <name val="&quot;Times New Roman&quot;"/>
       <family val="0"/>
       <charset val="1"/>
@@ -709,6 +715,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="&quot;Times New Roman&quot;"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -794,6 +806,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -806,20 +830,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -841,11 +853,11 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C160" activeCellId="0" sqref="C160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="22.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="22.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.57"/>
@@ -2102,9 +2114,7 @@
     </row>
     <row r="88" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1"/>
-      <c r="B88" s="1" t="n">
-        <v>9</v>
-      </c>
+      <c r="B88" s="1"/>
       <c r="C88" s="2" t="s">
         <v>61</v>
       </c>
@@ -2230,8 +2240,12 @@
     </row>
     <row r="97" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="4"/>
+      <c r="B97" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -2243,7 +2257,9 @@
     <row r="98" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-      <c r="C98" s="4"/>
+      <c r="C98" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -2255,7 +2271,9 @@
     <row r="99" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
-      <c r="C99" s="4"/>
+      <c r="C99" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -2266,11 +2284,9 @@
     </row>
     <row r="100" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1"/>
-      <c r="B100" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>66</v>
+      <c r="B100" s="1"/>
+      <c r="C100" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -2283,7 +2299,7 @@
     <row r="101" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
-      <c r="C101" s="4"/>
+      <c r="C101" s="9"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -2293,12 +2309,10 @@
       <c r="J101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>67</v>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -2309,12 +2323,10 @@
       <c r="J102" s="1"/>
     </row>
     <row r="103" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>68</v>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -2325,12 +2337,10 @@
       <c r="J103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>69</v>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -2341,12 +2351,10 @@
       <c r="J104" s="1"/>
     </row>
     <row r="105" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>52</v>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -2359,7 +2367,7 @@
     <row r="106" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="4"/>
+      <c r="C106" s="8"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -2370,12 +2378,8 @@
     </row>
     <row r="107" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1"/>
-      <c r="B107" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="8"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -2387,9 +2391,7 @@
     <row r="108" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
-      <c r="C108" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="C108" s="8"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -2401,9 +2403,7 @@
     <row r="109" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="C109" s="4"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -2414,9 +2414,11 @@
     </row>
     <row r="110" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
+      <c r="B110" s="1" t="n">
+        <v>10</v>
+      </c>
       <c r="C110" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -2429,9 +2431,7 @@
     <row r="111" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
-      <c r="C111" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C111" s="4"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -2441,9 +2441,13 @@
       <c r="J111" s="1"/>
     </row>
     <row r="112" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="4"/>
+      <c r="A112" s="3"/>
+      <c r="B112" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -2453,9 +2457,13 @@
       <c r="J112" s="1"/>
     </row>
     <row r="113" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="4"/>
+      <c r="A113" s="3"/>
+      <c r="B113" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -2465,12 +2473,12 @@
       <c r="J113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1" t="n">
-        <v>12</v>
+      <c r="A114" s="3"/>
+      <c r="B114" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -2481,9 +2489,13 @@
       <c r="J114" s="1"/>
     </row>
     <row r="115" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="4"/>
+      <c r="A115" s="3"/>
+      <c r="B115" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -2495,9 +2507,7 @@
     <row r="116" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
-      <c r="C116" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="C116" s="4"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -2508,9 +2518,11 @@
     </row>
     <row r="117" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
+      <c r="B117" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="C117" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -2524,7 +2536,7 @@
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -2538,7 +2550,7 @@
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -2551,7 +2563,9 @@
     <row r="120" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="4"/>
+      <c r="C120" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -2562,11 +2576,9 @@
     </row>
     <row r="121" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
-      <c r="B121" s="1" t="n">
-        <v>13</v>
-      </c>
+      <c r="B121" s="1"/>
       <c r="C121" s="4" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -2579,9 +2591,7 @@
     <row r="122" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
-      <c r="C122" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="C122" s="4"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -2593,9 +2603,7 @@
     <row r="123" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
-      <c r="C123" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="C123" s="4"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -2606,7 +2614,9 @@
     </row>
     <row r="124" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
+      <c r="B124" s="1" t="n">
+        <v>12</v>
+      </c>
       <c r="C124" s="4" t="s">
         <v>82</v>
       </c>
@@ -2621,9 +2631,7 @@
     <row r="125" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
-      <c r="C125" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C125" s="4"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -2635,7 +2643,9 @@
     <row r="126" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
-      <c r="C126" s="4"/>
+      <c r="C126" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -2647,7 +2657,9 @@
     <row r="127" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
-      <c r="C127" s="4"/>
+      <c r="C127" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -2658,11 +2670,9 @@
     </row>
     <row r="128" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
-      <c r="B128" s="1" t="n">
-        <v>14</v>
-      </c>
+      <c r="B128" s="1"/>
       <c r="C128" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -2676,7 +2686,7 @@
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -2689,9 +2699,7 @@
     <row r="130" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
-      <c r="C130" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="C130" s="4"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -2702,9 +2710,11 @@
     </row>
     <row r="131" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
+      <c r="B131" s="1" t="n">
+        <v>13</v>
+      </c>
       <c r="C131" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -2718,7 +2728,7 @@
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -2731,7 +2741,9 @@
     <row r="133" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
-      <c r="C133" s="4"/>
+      <c r="C133" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -2743,7 +2755,9 @@
     <row r="134" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
-      <c r="C134" s="4"/>
+      <c r="C134" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
@@ -2754,11 +2768,9 @@
     </row>
     <row r="135" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="1"/>
-      <c r="B135" s="1" t="n">
-        <v>15</v>
-      </c>
+      <c r="B135" s="1"/>
       <c r="C135" s="4" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -2771,9 +2783,7 @@
     <row r="136" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
-      <c r="C136" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="C136" s="4"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -2785,9 +2795,7 @@
     <row r="137" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
-      <c r="C137" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="C137" s="4"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -2798,9 +2806,11 @@
     </row>
     <row r="138" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
+      <c r="B138" s="1" t="n">
+        <v>14</v>
+      </c>
       <c r="C138" s="4" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
@@ -2814,7 +2824,7 @@
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -2827,7 +2837,9 @@
     <row r="140" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
-      <c r="C140" s="4"/>
+      <c r="C140" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -2839,7 +2851,9 @@
     <row r="141" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
-      <c r="C141" s="4"/>
+      <c r="C141" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -2850,11 +2864,9 @@
     </row>
     <row r="142" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="1"/>
-      <c r="B142" s="1" t="n">
-        <v>16</v>
-      </c>
+      <c r="B142" s="1"/>
       <c r="C142" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -2867,9 +2879,7 @@
     <row r="143" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
-      <c r="C143" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="C143" s="4"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
@@ -2881,9 +2891,7 @@
     <row r="144" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
-      <c r="C144" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="C144" s="4"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
@@ -2894,9 +2902,11 @@
     </row>
     <row r="145" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
+      <c r="B145" s="1" t="n">
+        <v>15</v>
+      </c>
       <c r="C145" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -2910,7 +2920,7 @@
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -2924,7 +2934,7 @@
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -2938,7 +2948,7 @@
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -2952,7 +2962,7 @@
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -2965,9 +2975,7 @@
     <row r="150" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
-      <c r="C150" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="C150" s="4"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
@@ -2979,9 +2987,7 @@
     <row r="151" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
-      <c r="C151" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="C151" s="4"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
@@ -2992,9 +2998,11 @@
     </row>
     <row r="152" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
+      <c r="B152" s="1" t="n">
+        <v>16</v>
+      </c>
       <c r="C152" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -3008,7 +3016,7 @@
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -3022,7 +3030,7 @@
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -3036,7 +3044,7 @@
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -3050,7 +3058,7 @@
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
@@ -3063,7 +3071,9 @@
     <row r="157" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
-      <c r="C157" s="4"/>
+      <c r="C157" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
@@ -3076,7 +3086,7 @@
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
@@ -3090,7 +3100,7 @@
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="4" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
@@ -3104,7 +3114,7 @@
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
@@ -3118,7 +3128,7 @@
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="4" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -3132,7 +3142,7 @@
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -3146,7 +3156,7 @@
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="4" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -3159,7 +3169,9 @@
     <row r="164" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
-      <c r="C164" s="4"/>
+      <c r="C164" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
@@ -3170,11 +3182,9 @@
     </row>
     <row r="165" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="1"/>
-      <c r="B165" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="B165" s="1"/>
       <c r="C165" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -3186,11 +3196,9 @@
     </row>
     <row r="166" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="1"/>
-      <c r="B166" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="B166" s="1"/>
       <c r="C166" s="4" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -3202,12 +3210,8 @@
     </row>
     <row r="167" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="1"/>
-      <c r="B167" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="B167" s="1"/>
+      <c r="C167" s="4"/>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
@@ -3218,11 +3222,9 @@
     </row>
     <row r="168" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
-      <c r="B168" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B168" s="1"/>
       <c r="C168" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
@@ -3235,7 +3237,9 @@
     <row r="169" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
-      <c r="C169" s="4"/>
+      <c r="C169" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
@@ -3247,7 +3251,9 @@
     <row r="170" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
-      <c r="C170" s="4"/>
+      <c r="C170" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
@@ -3258,11 +3264,9 @@
     </row>
     <row r="171" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
-      <c r="B171" s="1" t="n">
-        <v>17</v>
-      </c>
+      <c r="B171" s="1"/>
       <c r="C171" s="4" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
@@ -3276,7 +3280,7 @@
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="4" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
@@ -3290,7 +3294,7 @@
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="4" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -3303,9 +3307,7 @@
     <row r="174" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
-      <c r="C174" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C174" s="4"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
@@ -3316,9 +3318,11 @@
     </row>
     <row r="175" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
+      <c r="B175" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="C175" s="4" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -3330,9 +3334,11 @@
     </row>
     <row r="176" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
+      <c r="B176" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="C176" s="4" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -3344,9 +3350,11 @@
     </row>
     <row r="177" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
+      <c r="B177" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="C177" s="4" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
@@ -3358,9 +3366,11 @@
     </row>
     <row r="178" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
+      <c r="B178" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="C178" s="4" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -3373,9 +3383,7 @@
     <row r="179" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
-      <c r="C179" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="C179" s="4"/>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
@@ -3387,9 +3395,7 @@
     <row r="180" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
-      <c r="C180" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="C180" s="4"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
@@ -3400,9 +3406,11 @@
     </row>
     <row r="181" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
+      <c r="B181" s="1" t="n">
+        <v>17</v>
+      </c>
       <c r="C181" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -3416,7 +3424,7 @@
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -3430,7 +3438,7 @@
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -3444,7 +3452,7 @@
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -3458,7 +3466,7 @@
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -3471,7 +3479,9 @@
     <row r="186" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
-      <c r="C186" s="4"/>
+      <c r="C186" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
@@ -3484,7 +3494,7 @@
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="4" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -3498,7 +3508,7 @@
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="4" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
@@ -3512,7 +3522,7 @@
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
@@ -3526,7 +3536,7 @@
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="4" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -3540,7 +3550,7 @@
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
@@ -3554,7 +3564,7 @@
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="4" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
@@ -3567,7 +3577,9 @@
     <row r="193" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
-      <c r="C193" s="4"/>
+      <c r="C193" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
       <c r="F193" s="1"/>
@@ -3580,7 +3592,7 @@
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -3594,7 +3606,7 @@
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -3607,9 +3619,7 @@
     <row r="196" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
-      <c r="C196" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="C196" s="4"/>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
       <c r="F196" s="1"/>
@@ -3622,7 +3632,7 @@
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="4" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -3635,7 +3645,9 @@
     <row r="198" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
-      <c r="C198" s="4"/>
+      <c r="C198" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
       <c r="F198" s="1"/>
@@ -3647,7 +3659,9 @@
     <row r="199" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
-      <c r="C199" s="4"/>
+      <c r="C199" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
       <c r="F199" s="1"/>
@@ -3658,11 +3672,9 @@
     </row>
     <row r="200" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="1"/>
-      <c r="B200" s="1" t="n">
-        <v>18</v>
-      </c>
+      <c r="B200" s="1"/>
       <c r="C200" s="4" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -3676,7 +3688,7 @@
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="4" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
@@ -3690,7 +3702,7 @@
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="4" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -3703,9 +3715,7 @@
     <row r="203" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
-      <c r="C203" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C203" s="4"/>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
       <c r="F203" s="1"/>
@@ -3718,7 +3728,7 @@
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="4" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
@@ -3732,7 +3742,7 @@
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="4" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -3746,7 +3756,7 @@
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="4" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -3760,7 +3770,7 @@
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="4" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -3773,9 +3783,7 @@
     <row r="208" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
-      <c r="C208" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="C208" s="4"/>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
       <c r="F208" s="1"/>
@@ -3787,9 +3795,7 @@
     <row r="209" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
-      <c r="C209" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="C209" s="4"/>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
       <c r="F209" s="1"/>
@@ -3800,9 +3806,11 @@
     </row>
     <row r="210" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
+      <c r="B210" s="1" t="n">
+        <v>18</v>
+      </c>
       <c r="C210" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D210" s="1"/>
       <c r="E210" s="1"/>
@@ -3816,7 +3824,7 @@
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
@@ -3829,7 +3837,9 @@
     <row r="212" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
-      <c r="C212" s="4"/>
+      <c r="C212" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
       <c r="F212" s="1"/>
@@ -3856,7 +3866,7 @@
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
@@ -3870,7 +3880,7 @@
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
@@ -3884,7 +3894,7 @@
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="4" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D216" s="1"/>
       <c r="E216" s="1"/>
@@ -3897,7 +3907,9 @@
     <row r="217" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
-      <c r="C217" s="4"/>
+      <c r="C217" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
       <c r="F217" s="1"/>
@@ -3910,7 +3922,7 @@
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D218" s="1"/>
       <c r="E218" s="1"/>
@@ -3924,7 +3936,7 @@
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
@@ -3938,7 +3950,7 @@
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
@@ -3952,7 +3964,7 @@
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="4" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
@@ -3965,9 +3977,7 @@
     <row r="222" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
-      <c r="C222" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="C222" s="4"/>
       <c r="D222" s="1"/>
       <c r="E222" s="1"/>
       <c r="F222" s="1"/>
@@ -3980,7 +3990,7 @@
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="4" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
@@ -3993,7 +4003,9 @@
     <row r="224" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
-      <c r="C224" s="4"/>
+      <c r="C224" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
       <c r="F224" s="1"/>
@@ -4006,7 +4018,7 @@
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="4" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
@@ -4020,7 +4032,7 @@
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
@@ -4033,9 +4045,7 @@
     <row r="227" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
-      <c r="C227" s="4" t="s">
-        <v>121</v>
-      </c>
+      <c r="C227" s="4"/>
       <c r="D227" s="1"/>
       <c r="E227" s="1"/>
       <c r="F227" s="1"/>
@@ -4048,7 +4058,7 @@
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="4" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D228" s="1"/>
       <c r="E228" s="1"/>
@@ -4061,7 +4071,9 @@
     <row r="229" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
-      <c r="C229" s="9"/>
+      <c r="C229" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="D229" s="1"/>
       <c r="E229" s="1"/>
       <c r="F229" s="1"/>
@@ -4072,11 +4084,9 @@
     </row>
     <row r="230" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="1"/>
-      <c r="B230" s="10" t="n">
-        <v>19</v>
-      </c>
-      <c r="C230" s="11" t="s">
-        <v>123</v>
+      <c r="B230" s="1"/>
+      <c r="C230" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="D230" s="1"/>
       <c r="E230" s="1"/>
@@ -4089,8 +4099,8 @@
     <row r="231" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
-      <c r="C231" s="11" t="s">
-        <v>124</v>
+      <c r="C231" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="D231" s="1"/>
       <c r="E231" s="1"/>
@@ -4103,8 +4113,8 @@
     <row r="232" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
-      <c r="C232" s="11" t="s">
-        <v>125</v>
+      <c r="C232" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D232" s="1"/>
       <c r="E232" s="1"/>
@@ -4117,8 +4127,8 @@
     <row r="233" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
-      <c r="C233" s="11" t="s">
-        <v>126</v>
+      <c r="C233" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D233" s="1"/>
       <c r="E233" s="1"/>
@@ -4131,9 +4141,7 @@
     <row r="234" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
-      <c r="C234" s="11" t="s">
-        <v>127</v>
-      </c>
+      <c r="C234" s="4"/>
       <c r="D234" s="1"/>
       <c r="E234" s="1"/>
       <c r="F234" s="1"/>
@@ -4145,8 +4153,8 @@
     <row r="235" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
-      <c r="C235" s="11" t="s">
-        <v>128</v>
+      <c r="C235" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="D235" s="1"/>
       <c r="E235" s="1"/>
@@ -4159,8 +4167,8 @@
     <row r="236" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
-      <c r="C236" s="11" t="s">
-        <v>129</v>
+      <c r="C236" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="D236" s="1"/>
       <c r="E236" s="1"/>
@@ -4173,8 +4181,8 @@
     <row r="237" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
-      <c r="C237" s="11" t="s">
-        <v>130</v>
+      <c r="C237" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="D237" s="1"/>
       <c r="E237" s="1"/>
@@ -4187,8 +4195,8 @@
     <row r="238" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
-      <c r="C238" s="11" t="s">
-        <v>38</v>
+      <c r="C238" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="D238" s="1"/>
       <c r="E238" s="1"/>
@@ -4201,9 +4209,7 @@
     <row r="239" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
-      <c r="C239" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="C239" s="12"/>
       <c r="D239" s="1"/>
       <c r="E239" s="1"/>
       <c r="F239" s="1"/>
@@ -4214,9 +4220,11 @@
     </row>
     <row r="240" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="1"/>
-      <c r="B240" s="1"/>
-      <c r="C240" s="11" t="s">
-        <v>131</v>
+      <c r="B240" s="13" t="n">
+        <v>19</v>
+      </c>
+      <c r="C240" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="D240" s="1"/>
       <c r="E240" s="1"/>
@@ -4229,8 +4237,8 @@
     <row r="241" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
-      <c r="C241" s="11" t="s">
-        <v>132</v>
+      <c r="C241" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="D241" s="1"/>
       <c r="E241" s="1"/>
@@ -4243,8 +4251,8 @@
     <row r="242" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
-      <c r="C242" s="11" t="s">
-        <v>133</v>
+      <c r="C242" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="D242" s="1"/>
       <c r="E242" s="1"/>
@@ -4257,8 +4265,8 @@
     <row r="243" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
-      <c r="C243" s="11" t="s">
-        <v>134</v>
+      <c r="C243" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="D243" s="1"/>
       <c r="E243" s="1"/>
@@ -4271,7 +4279,9 @@
     <row r="244" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
-      <c r="C244" s="11"/>
+      <c r="C244" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="D244" s="1"/>
       <c r="E244" s="1"/>
       <c r="F244" s="1"/>
@@ -4283,7 +4293,9 @@
     <row r="245" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
-      <c r="C245" s="11"/>
+      <c r="C245" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="D245" s="1"/>
       <c r="E245" s="1"/>
       <c r="F245" s="1"/>
@@ -4295,7 +4307,9 @@
     <row r="246" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
-      <c r="C246" s="11"/>
+      <c r="C246" s="14" t="s">
+        <v>141</v>
+      </c>
       <c r="D246" s="1"/>
       <c r="E246" s="1"/>
       <c r="F246" s="1"/>
@@ -4306,11 +4320,9 @@
     </row>
     <row r="247" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="1"/>
-      <c r="B247" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="C247" s="12" t="s">
-        <v>125</v>
+      <c r="B247" s="1"/>
+      <c r="C247" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="D247" s="1"/>
       <c r="E247" s="1"/>
@@ -4323,8 +4335,8 @@
     <row r="248" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
-      <c r="C248" s="12" t="s">
-        <v>126</v>
+      <c r="C248" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="D248" s="1"/>
       <c r="E248" s="1"/>
@@ -4337,8 +4349,8 @@
     <row r="249" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
-      <c r="C249" s="12" t="s">
-        <v>135</v>
+      <c r="C249" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="D249" s="1"/>
       <c r="E249" s="1"/>
@@ -4351,8 +4363,8 @@
     <row r="250" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
-      <c r="C250" s="12" t="s">
-        <v>38</v>
+      <c r="C250" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="D250" s="1"/>
       <c r="E250" s="1"/>
@@ -4365,8 +4377,8 @@
     <row r="251" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
-      <c r="C251" s="12" t="s">
-        <v>38</v>
+      <c r="C251" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="D251" s="1"/>
       <c r="E251" s="1"/>
@@ -4379,8 +4391,8 @@
     <row r="252" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="1"/>
       <c r="B252" s="1"/>
-      <c r="C252" s="12" t="s">
-        <v>136</v>
+      <c r="C252" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="D252" s="1"/>
       <c r="E252" s="1"/>
@@ -4393,8 +4405,8 @@
     <row r="253" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="1"/>
       <c r="B253" s="1"/>
-      <c r="C253" s="12" t="s">
-        <v>137</v>
+      <c r="C253" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="D253" s="1"/>
       <c r="E253" s="1"/>
@@ -4407,9 +4419,7 @@
     <row r="254" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="1"/>
       <c r="B254" s="1"/>
-      <c r="C254" s="12" t="s">
-        <v>138</v>
-      </c>
+      <c r="C254" s="14"/>
       <c r="D254" s="1"/>
       <c r="E254" s="1"/>
       <c r="F254" s="1"/>
@@ -4421,9 +4431,7 @@
     <row r="255" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="1"/>
       <c r="B255" s="1"/>
-      <c r="C255" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="C255" s="14"/>
       <c r="D255" s="1"/>
       <c r="E255" s="1"/>
       <c r="F255" s="1"/>
@@ -4435,9 +4443,7 @@
     <row r="256" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="1"/>
       <c r="B256" s="1"/>
-      <c r="C256" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="C256" s="14"/>
       <c r="D256" s="1"/>
       <c r="E256" s="1"/>
       <c r="F256" s="1"/>
@@ -4448,9 +4454,11 @@
     </row>
     <row r="257" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="1"/>
-      <c r="B257" s="1"/>
-      <c r="C257" s="12" t="s">
-        <v>139</v>
+      <c r="B257" s="13" t="n">
+        <v>20</v>
+      </c>
+      <c r="C257" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="D257" s="1"/>
       <c r="E257" s="1"/>
@@ -4463,8 +4471,8 @@
     <row r="258" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="1"/>
       <c r="B258" s="1"/>
-      <c r="C258" s="12" t="s">
-        <v>140</v>
+      <c r="C258" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="D258" s="1"/>
       <c r="E258" s="1"/>
@@ -4477,8 +4485,8 @@
     <row r="259" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="1"/>
       <c r="B259" s="1"/>
-      <c r="C259" s="12" t="s">
-        <v>141</v>
+      <c r="C259" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="D259" s="1"/>
       <c r="E259" s="1"/>
@@ -4491,7 +4499,7 @@
     <row r="260" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="1"/>
       <c r="B260" s="1"/>
-      <c r="C260" s="12" t="s">
+      <c r="C260" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D260" s="1"/>
@@ -4505,7 +4513,7 @@
     <row r="261" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="1"/>
       <c r="B261" s="1"/>
-      <c r="C261" s="12" t="s">
+      <c r="C261" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D261" s="1"/>
@@ -4519,8 +4527,8 @@
     <row r="262" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="1"/>
       <c r="B262" s="1"/>
-      <c r="C262" s="12" t="s">
-        <v>142</v>
+      <c r="C262" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="D262" s="1"/>
       <c r="E262" s="1"/>
@@ -4533,10 +4541,10 @@
     <row r="263" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="1"/>
       <c r="B263" s="1"/>
-      <c r="C263" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D263" s="10"/>
+      <c r="C263" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D263" s="1"/>
       <c r="E263" s="1"/>
       <c r="F263" s="1"/>
       <c r="G263" s="1"/>
@@ -4547,8 +4555,8 @@
     <row r="264" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="1"/>
       <c r="B264" s="1"/>
-      <c r="C264" s="12" t="s">
-        <v>144</v>
+      <c r="C264" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="D264" s="1"/>
       <c r="E264" s="1"/>
@@ -4561,8 +4569,8 @@
     <row r="265" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="1"/>
       <c r="B265" s="1"/>
-      <c r="C265" s="12" t="s">
-        <v>145</v>
+      <c r="C265" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D265" s="1"/>
       <c r="E265" s="1"/>
@@ -4575,7 +4583,9 @@
     <row r="266" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="1"/>
       <c r="B266" s="1"/>
-      <c r="C266" s="12"/>
+      <c r="C266" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D266" s="1"/>
       <c r="E266" s="1"/>
       <c r="F266" s="1"/>
@@ -4587,7 +4597,9 @@
     <row r="267" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="1"/>
       <c r="B267" s="1"/>
-      <c r="C267" s="12"/>
+      <c r="C267" s="9" t="s">
+        <v>151</v>
+      </c>
       <c r="D267" s="1"/>
       <c r="E267" s="1"/>
       <c r="F267" s="1"/>
@@ -4599,8 +4611,8 @@
     <row r="268" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="1"/>
       <c r="B268" s="1"/>
-      <c r="C268" s="13" t="s">
-        <v>146</v>
+      <c r="C268" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="D268" s="1"/>
       <c r="E268" s="1"/>
@@ -4613,8 +4625,8 @@
     <row r="269" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="1"/>
       <c r="B269" s="1"/>
-      <c r="C269" s="13" t="s">
-        <v>147</v>
+      <c r="C269" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="D269" s="1"/>
       <c r="E269" s="1"/>
@@ -4627,8 +4639,8 @@
     <row r="270" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="1"/>
       <c r="B270" s="1"/>
-      <c r="C270" s="13" t="s">
-        <v>148</v>
+      <c r="C270" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D270" s="1"/>
       <c r="E270" s="1"/>
@@ -4641,8 +4653,8 @@
     <row r="271" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="1"/>
       <c r="B271" s="1"/>
-      <c r="C271" s="13" t="s">
-        <v>149</v>
+      <c r="C271" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D271" s="1"/>
       <c r="E271" s="1"/>
@@ -4655,7 +4667,9 @@
     <row r="272" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="1"/>
       <c r="B272" s="1"/>
-      <c r="C272" s="12"/>
+      <c r="C272" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="D272" s="1"/>
       <c r="E272" s="1"/>
       <c r="F272" s="1"/>
@@ -4667,10 +4681,10 @@
     <row r="273" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="1"/>
       <c r="B273" s="1"/>
-      <c r="C273" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D273" s="1"/>
+      <c r="C273" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D273" s="13"/>
       <c r="E273" s="1"/>
       <c r="F273" s="1"/>
       <c r="G273" s="1"/>
@@ -4681,10 +4695,10 @@
     <row r="274" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="1"/>
       <c r="B274" s="1"/>
-      <c r="C274" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="D274" s="10"/>
+      <c r="C274" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D274" s="1"/>
       <c r="E274" s="1"/>
       <c r="F274" s="1"/>
       <c r="G274" s="1"/>
@@ -4695,8 +4709,8 @@
     <row r="275" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="1"/>
       <c r="B275" s="1"/>
-      <c r="C275" s="14" t="s">
-        <v>152</v>
+      <c r="C275" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="D275" s="1"/>
       <c r="E275" s="1"/>
@@ -4709,9 +4723,7 @@
     <row r="276" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="1"/>
       <c r="B276" s="1"/>
-      <c r="C276" s="14" t="s">
-        <v>153</v>
-      </c>
+      <c r="C276" s="9"/>
       <c r="D276" s="1"/>
       <c r="E276" s="1"/>
       <c r="F276" s="1"/>
@@ -4723,7 +4735,7 @@
     <row r="277" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="1"/>
       <c r="B277" s="1"/>
-      <c r="C277" s="12"/>
+      <c r="C277" s="9"/>
       <c r="D277" s="1"/>
       <c r="E277" s="1"/>
       <c r="F277" s="1"/>
@@ -4734,11 +4746,11 @@
     </row>
     <row r="278" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="1"/>
-      <c r="B278" s="10" t="n">
+      <c r="B278" s="13" t="n">
         <v>21</v>
       </c>
-      <c r="C278" s="12" t="s">
-        <v>154</v>
+      <c r="C278" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="D278" s="1"/>
       <c r="E278" s="1"/>
@@ -4751,8 +4763,8 @@
     <row r="279" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="1"/>
       <c r="B279" s="1"/>
-      <c r="C279" s="12" t="s">
-        <v>155</v>
+      <c r="C279" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="D279" s="1"/>
       <c r="E279" s="1"/>
@@ -4765,8 +4777,8 @@
     <row r="280" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="1"/>
       <c r="B280" s="1"/>
-      <c r="C280" s="12" t="s">
-        <v>126</v>
+      <c r="C280" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="D280" s="1"/>
       <c r="E280" s="1"/>
@@ -4779,8 +4791,8 @@
     <row r="281" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="1"/>
       <c r="B281" s="1"/>
-      <c r="C281" s="12" t="s">
-        <v>156</v>
+      <c r="C281" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="D281" s="1"/>
       <c r="E281" s="1"/>
@@ -4793,8 +4805,8 @@
     <row r="282" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="1"/>
       <c r="B282" s="1"/>
-      <c r="C282" s="12" t="s">
-        <v>157</v>
+      <c r="C282" s="9" t="s">
+        <v>161</v>
       </c>
       <c r="D282" s="1"/>
       <c r="E282" s="1"/>
@@ -4807,8 +4819,8 @@
     <row r="283" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="1"/>
       <c r="B283" s="1"/>
-      <c r="C283" s="12" t="s">
-        <v>158</v>
+      <c r="C283" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="D283" s="1"/>
       <c r="E283" s="1"/>
@@ -4821,8 +4833,8 @@
     <row r="284" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="1"/>
       <c r="B284" s="1"/>
-      <c r="C284" s="12" t="s">
-        <v>159</v>
+      <c r="C284" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="D284" s="1"/>
       <c r="E284" s="1"/>
@@ -4835,7 +4847,7 @@
     <row r="285" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="1"/>
       <c r="B285" s="1"/>
-      <c r="C285" s="12" t="s">
+      <c r="C285" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D285" s="1"/>
@@ -4849,8 +4861,8 @@
     <row r="286" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="1"/>
       <c r="B286" s="1"/>
-      <c r="C286" s="12" t="s">
-        <v>160</v>
+      <c r="C286" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="D286" s="1"/>
       <c r="E286" s="1"/>
@@ -4863,8 +4875,8 @@
     <row r="287" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="1"/>
       <c r="B287" s="1"/>
-      <c r="C287" s="12" t="s">
-        <v>161</v>
+      <c r="C287" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="D287" s="1"/>
       <c r="E287" s="1"/>
@@ -4877,7 +4889,7 @@
     <row r="288" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="1"/>
       <c r="B288" s="1"/>
-      <c r="C288" s="12" t="s">
+      <c r="C288" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D288" s="1"/>
@@ -4891,7 +4903,7 @@
     <row r="289" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="1"/>
       <c r="B289" s="1"/>
-      <c r="C289" s="12" t="s">
+      <c r="C289" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D289" s="1"/>
@@ -4905,8 +4917,8 @@
     <row r="290" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="1"/>
       <c r="B290" s="1"/>
-      <c r="C290" s="12" t="s">
-        <v>162</v>
+      <c r="C290" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="D290" s="1"/>
       <c r="E290" s="1"/>
@@ -4919,8 +4931,8 @@
     <row r="291" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="1"/>
       <c r="B291" s="1"/>
-      <c r="C291" s="12" t="s">
-        <v>163</v>
+      <c r="C291" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="D291" s="1"/>
       <c r="E291" s="1"/>
@@ -4933,7 +4945,7 @@
     <row r="292" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="1"/>
       <c r="B292" s="1"/>
-      <c r="C292" s="12" t="s">
+      <c r="C292" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D292" s="1"/>
@@ -4947,8 +4959,8 @@
     <row r="293" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="1"/>
       <c r="B293" s="1"/>
-      <c r="C293" s="12" t="s">
-        <v>164</v>
+      <c r="C293" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="D293" s="1"/>
       <c r="E293" s="1"/>
@@ -4961,8 +4973,8 @@
     <row r="294" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="1"/>
       <c r="B294" s="1"/>
-      <c r="C294" s="12" t="s">
-        <v>163</v>
+      <c r="C294" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="D294" s="1"/>
       <c r="E294" s="1"/>
@@ -4975,7 +4987,7 @@
     <row r="295" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="1"/>
       <c r="B295" s="1"/>
-      <c r="C295" s="12" t="s">
+      <c r="C295" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D295" s="1"/>
@@ -4989,8 +5001,8 @@
     <row r="296" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="1"/>
       <c r="B296" s="1"/>
-      <c r="C296" s="12" t="s">
-        <v>165</v>
+      <c r="C296" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="D296" s="1"/>
       <c r="E296" s="1"/>
@@ -5003,8 +5015,8 @@
     <row r="297" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="1"/>
       <c r="B297" s="1"/>
-      <c r="C297" s="12" t="s">
-        <v>166</v>
+      <c r="C297" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="D297" s="1"/>
       <c r="E297" s="1"/>
@@ -5017,10 +5029,10 @@
     <row r="298" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="1"/>
       <c r="B298" s="1"/>
-      <c r="C298" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="D298" s="10"/>
+      <c r="C298" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D298" s="13"/>
       <c r="E298" s="1"/>
       <c r="F298" s="1"/>
       <c r="G298" s="1"/>
@@ -5031,8 +5043,8 @@
     <row r="299" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="1"/>
       <c r="B299" s="1"/>
-      <c r="C299" s="12" t="s">
-        <v>168</v>
+      <c r="C299" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="D299" s="1"/>
       <c r="E299" s="1"/>
@@ -5045,7 +5057,7 @@
     <row r="300" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="1"/>
       <c r="B300" s="1"/>
-      <c r="C300" s="12"/>
+      <c r="C300" s="9"/>
       <c r="D300" s="1"/>
       <c r="E300" s="1"/>
       <c r="F300" s="1"/>
@@ -5057,7 +5069,7 @@
     <row r="301" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="1"/>
       <c r="B301" s="1"/>
-      <c r="C301" s="12"/>
+      <c r="C301" s="9"/>
       <c r="D301" s="1"/>
       <c r="E301" s="1"/>
       <c r="F301" s="1"/>
@@ -5068,11 +5080,11 @@
     </row>
     <row r="302" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="1"/>
-      <c r="B302" s="10" t="n">
+      <c r="B302" s="13" t="n">
         <v>22</v>
       </c>
-      <c r="C302" s="12" t="s">
-        <v>169</v>
+      <c r="C302" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="D302" s="1"/>
       <c r="E302" s="1"/>
@@ -5085,8 +5097,8 @@
     <row r="303" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="1"/>
       <c r="B303" s="1"/>
-      <c r="C303" s="12" t="s">
-        <v>170</v>
+      <c r="C303" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="D303" s="1"/>
       <c r="E303" s="1"/>
@@ -5099,8 +5111,8 @@
     <row r="304" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
-      <c r="C304" s="12" t="s">
-        <v>171</v>
+      <c r="C304" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="D304" s="1"/>
       <c r="E304" s="1"/>
@@ -5113,7 +5125,7 @@
     <row r="305" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
-      <c r="C305" s="12" t="s">
+      <c r="C305" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D305" s="1"/>
@@ -5127,8 +5139,8 @@
     <row r="306" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
-      <c r="C306" s="12" t="s">
-        <v>172</v>
+      <c r="C306" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="D306" s="1"/>
       <c r="E306" s="1"/>
@@ -5141,8 +5153,8 @@
     <row r="307" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="1"/>
       <c r="B307" s="1"/>
-      <c r="C307" s="12" t="s">
-        <v>173</v>
+      <c r="C307" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="D307" s="1"/>
       <c r="E307" s="1"/>
@@ -5155,8 +5167,8 @@
     <row r="308" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="1"/>
       <c r="B308" s="1"/>
-      <c r="C308" s="12" t="s">
-        <v>174</v>
+      <c r="C308" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="D308" s="1"/>
       <c r="E308" s="1"/>
@@ -5169,7 +5181,7 @@
     <row r="309" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="1"/>
       <c r="B309" s="1"/>
-      <c r="C309" s="12" t="s">
+      <c r="C309" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D309" s="1"/>
@@ -5183,8 +5195,8 @@
     <row r="310" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="1"/>
       <c r="B310" s="1"/>
-      <c r="C310" s="12" t="s">
-        <v>175</v>
+      <c r="C310" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="D310" s="1"/>
       <c r="E310" s="1"/>
@@ -5197,8 +5209,8 @@
     <row r="311" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="1"/>
       <c r="B311" s="1"/>
-      <c r="C311" s="12" t="s">
-        <v>176</v>
+      <c r="C311" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="D311" s="1"/>
       <c r="E311" s="1"/>
@@ -5211,7 +5223,7 @@
     <row r="312" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="1"/>
       <c r="B312" s="1"/>
-      <c r="C312" s="12" t="s">
+      <c r="C312" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D312" s="1"/>
@@ -5225,8 +5237,8 @@
     <row r="313" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="1"/>
       <c r="B313" s="1"/>
-      <c r="C313" s="12" t="s">
-        <v>160</v>
+      <c r="C313" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="D313" s="1"/>
       <c r="E313" s="1"/>
@@ -5239,8 +5251,8 @@
     <row r="314" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="1"/>
       <c r="B314" s="1"/>
-      <c r="C314" s="12" t="s">
-        <v>177</v>
+      <c r="C314" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="D314" s="1"/>
       <c r="E314" s="1"/>
@@ -5253,7 +5265,7 @@
     <row r="315" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="1"/>
       <c r="B315" s="1"/>
-      <c r="C315" s="12" t="s">
+      <c r="C315" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D315" s="1"/>
@@ -5267,7 +5279,7 @@
     <row r="316" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="1"/>
       <c r="B316" s="1"/>
-      <c r="C316" s="12" t="s">
+      <c r="C316" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D316" s="1"/>
@@ -5281,8 +5293,8 @@
     <row r="317" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="1"/>
       <c r="B317" s="1"/>
-      <c r="C317" s="12" t="s">
-        <v>178</v>
+      <c r="C317" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="D317" s="1"/>
       <c r="E317" s="1"/>
@@ -5295,8 +5307,8 @@
     <row r="318" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="1"/>
       <c r="B318" s="1"/>
-      <c r="C318" s="12" t="s">
-        <v>179</v>
+      <c r="C318" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="D318" s="1"/>
       <c r="E318" s="1"/>
@@ -5309,8 +5321,8 @@
     <row r="319" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="1"/>
       <c r="B319" s="1"/>
-      <c r="C319" s="12" t="s">
-        <v>180</v>
+      <c r="C319" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="D319" s="1"/>
       <c r="E319" s="1"/>
@@ -5323,10 +5335,10 @@
     <row r="320" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="1"/>
       <c r="B320" s="1"/>
-      <c r="C320" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="D320" s="10"/>
+      <c r="C320" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D320" s="13"/>
       <c r="E320" s="1"/>
       <c r="F320" s="1"/>
       <c r="G320" s="1"/>
@@ -5337,7 +5349,7 @@
     <row r="321" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="1"/>
       <c r="B321" s="1"/>
-      <c r="C321" s="12"/>
+      <c r="C321" s="9"/>
       <c r="D321" s="1"/>
       <c r="E321" s="1"/>
       <c r="F321" s="1"/>
@@ -5348,11 +5360,11 @@
     </row>
     <row r="322" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="1"/>
-      <c r="B322" s="10" t="n">
+      <c r="B322" s="13" t="n">
         <v>23</v>
       </c>
-      <c r="C322" s="12" t="s">
-        <v>182</v>
+      <c r="C322" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="D322" s="1"/>
       <c r="E322" s="1"/>
@@ -5365,8 +5377,8 @@
     <row r="323" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="1"/>
       <c r="B323" s="1"/>
-      <c r="C323" s="12" t="s">
-        <v>183</v>
+      <c r="C323" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="D323" s="1"/>
       <c r="E323" s="1"/>
@@ -5379,10 +5391,10 @@
     <row r="324" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="1"/>
       <c r="B324" s="1"/>
-      <c r="C324" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D324" s="10"/>
+      <c r="C324" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D324" s="13"/>
       <c r="E324" s="1"/>
       <c r="F324" s="1"/>
       <c r="G324" s="1"/>
@@ -5393,8 +5405,8 @@
     <row r="325" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="1"/>
       <c r="B325" s="1"/>
-      <c r="C325" s="12" t="s">
-        <v>185</v>
+      <c r="C325" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="D325" s="1"/>
       <c r="E325" s="1"/>
@@ -5407,8 +5419,8 @@
     <row r="326" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="1"/>
       <c r="B326" s="1"/>
-      <c r="C326" s="12" t="s">
-        <v>186</v>
+      <c r="C326" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="D326" s="1"/>
       <c r="E326" s="1"/>
@@ -5421,7 +5433,7 @@
     <row r="327" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="1"/>
       <c r="B327" s="1"/>
-      <c r="C327" s="12"/>
+      <c r="C327" s="9"/>
       <c r="D327" s="1"/>
       <c r="E327" s="1"/>
       <c r="F327" s="1"/>
@@ -5433,7 +5445,7 @@
     <row r="328" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="1"/>
       <c r="B328" s="1"/>
-      <c r="C328" s="12"/>
+      <c r="C328" s="9"/>
       <c r="D328" s="1"/>
       <c r="E328" s="1"/>
       <c r="F328" s="1"/>
@@ -5444,11 +5456,11 @@
     </row>
     <row r="329" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="1"/>
-      <c r="B329" s="10" t="n">
+      <c r="B329" s="13" t="n">
         <v>24</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D329" s="1"/>
       <c r="E329" s="1"/>
@@ -5460,9 +5472,9 @@
     </row>
     <row r="330" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="1"/>
-      <c r="B330" s="10"/>
+      <c r="B330" s="13"/>
       <c r="C330" s="4" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="D330" s="1"/>
       <c r="E330" s="1"/>
@@ -5474,9 +5486,9 @@
     </row>
     <row r="331" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="1"/>
-      <c r="B331" s="10"/>
+      <c r="B331" s="13"/>
       <c r="C331" s="4" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D331" s="1"/>
       <c r="E331" s="1"/>
@@ -5488,9 +5500,9 @@
     </row>
     <row r="332" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="1"/>
-      <c r="B332" s="10"/>
+      <c r="B332" s="13"/>
       <c r="C332" s="4" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D332" s="1"/>
       <c r="E332" s="1"/>
@@ -5502,9 +5514,9 @@
     </row>
     <row r="333" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="1"/>
-      <c r="B333" s="10"/>
+      <c r="B333" s="13"/>
       <c r="C333" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D333" s="1"/>
       <c r="E333" s="1"/>
@@ -5516,9 +5528,9 @@
     </row>
     <row r="334" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="1"/>
-      <c r="B334" s="10"/>
+      <c r="B334" s="13"/>
       <c r="C334" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D334" s="1"/>
       <c r="E334" s="1"/>
@@ -5530,9 +5542,9 @@
     </row>
     <row r="335" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="1"/>
-      <c r="B335" s="10"/>
+      <c r="B335" s="13"/>
       <c r="C335" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D335" s="1"/>
       <c r="E335" s="1"/>
@@ -5544,9 +5556,9 @@
     </row>
     <row r="336" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="1"/>
-      <c r="B336" s="10"/>
+      <c r="B336" s="13"/>
       <c r="C336" s="4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D336" s="1"/>
       <c r="E336" s="1"/>
@@ -5558,9 +5570,9 @@
     </row>
     <row r="337" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="1"/>
-      <c r="B337" s="10"/>
+      <c r="B337" s="13"/>
       <c r="C337" s="4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D337" s="1"/>
       <c r="E337" s="1"/>
@@ -5572,9 +5584,9 @@
     </row>
     <row r="338" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="1"/>
-      <c r="B338" s="10"/>
+      <c r="B338" s="13"/>
       <c r="C338" s="4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D338" s="1"/>
       <c r="E338" s="1"/>
@@ -5586,9 +5598,9 @@
     </row>
     <row r="339" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="1"/>
-      <c r="B339" s="10"/>
+      <c r="B339" s="13"/>
       <c r="C339" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D339" s="1"/>
       <c r="E339" s="1"/>
@@ -5602,9 +5614,9 @@
       <c r="A340" s="1"/>
       <c r="B340" s="1"/>
       <c r="C340" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D340" s="10"/>
+        <v>198</v>
+      </c>
+      <c r="D340" s="13"/>
       <c r="E340" s="1"/>
       <c r="F340" s="1"/>
       <c r="G340" s="1"/>
@@ -5615,7 +5627,7 @@
     <row r="341" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="1"/>
       <c r="B341" s="1"/>
-      <c r="C341" s="12"/>
+      <c r="C341" s="9"/>
       <c r="D341" s="1"/>
       <c r="E341" s="1"/>
       <c r="F341" s="1"/>
@@ -5627,7 +5639,7 @@
     <row r="342" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="1"/>
       <c r="B342" s="1"/>
-      <c r="C342" s="12"/>
+      <c r="C342" s="9"/>
       <c r="D342" s="1"/>
       <c r="E342" s="1"/>
       <c r="F342" s="1"/>
@@ -5638,11 +5650,11 @@
     </row>
     <row r="343" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="1"/>
-      <c r="B343" s="10" t="n">
+      <c r="B343" s="13" t="n">
         <v>25</v>
       </c>
-      <c r="C343" s="12" t="s">
-        <v>195</v>
+      <c r="C343" s="9" t="s">
+        <v>199</v>
       </c>
       <c r="D343" s="1"/>
       <c r="E343" s="1"/>
@@ -5655,7 +5667,7 @@
     <row r="344" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="1"/>
       <c r="B344" s="1"/>
-      <c r="C344" s="12"/>
+      <c r="C344" s="9"/>
       <c r="D344" s="1"/>
       <c r="E344" s="1"/>
       <c r="F344" s="1"/>
@@ -5666,11 +5678,11 @@
     </row>
     <row r="345" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="1"/>
-      <c r="B345" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C345" s="12" t="s">
-        <v>197</v>
+      <c r="B345" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C345" s="9" t="s">
+        <v>201</v>
       </c>
       <c r="D345" s="1"/>
       <c r="E345" s="1"/>
@@ -5682,11 +5694,11 @@
     </row>
     <row r="346" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="1"/>
-      <c r="B346" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C346" s="12" t="s">
-        <v>199</v>
+      <c r="B346" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C346" s="9" t="s">
+        <v>203</v>
       </c>
       <c r="D346" s="1"/>
       <c r="E346" s="1"/>
@@ -5698,11 +5710,11 @@
     </row>
     <row r="347" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="1"/>
-      <c r="B347" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C347" s="12" t="s">
-        <v>201</v>
+      <c r="B347" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C347" s="9" t="s">
+        <v>205</v>
       </c>
       <c r="D347" s="1"/>
       <c r="E347" s="1"/>
@@ -5714,13 +5726,13 @@
     </row>
     <row r="348" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="1"/>
-      <c r="B348" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C348" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D348" s="10"/>
+      <c r="B348" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C348" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D348" s="13"/>
       <c r="E348" s="1"/>
       <c r="F348" s="1"/>
       <c r="G348" s="1"/>
@@ -5731,7 +5743,7 @@
     <row r="349" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="1"/>
       <c r="B349" s="1"/>
-      <c r="C349" s="12"/>
+      <c r="C349" s="9"/>
       <c r="D349" s="1"/>
       <c r="E349" s="1"/>
       <c r="F349" s="1"/>
@@ -5743,7 +5755,7 @@
     <row r="350" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="1"/>
       <c r="B350" s="1"/>
-      <c r="C350" s="12"/>
+      <c r="C350" s="9"/>
       <c r="D350" s="1"/>
       <c r="E350" s="1"/>
       <c r="F350" s="1"/>
@@ -5755,7 +5767,7 @@
     <row r="351" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="1"/>
       <c r="B351" s="1"/>
-      <c r="C351" s="12"/>
+      <c r="C351" s="9"/>
       <c r="D351" s="1"/>
       <c r="E351" s="1"/>
       <c r="F351" s="1"/>
@@ -5767,7 +5779,7 @@
     <row r="352" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="1"/>
       <c r="B352" s="1"/>
-      <c r="C352" s="12"/>
+      <c r="C352" s="9"/>
       <c r="D352" s="1"/>
       <c r="E352" s="1"/>
       <c r="F352" s="1"/>
@@ -5779,7 +5791,7 @@
     <row r="353" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="1"/>
       <c r="B353" s="1"/>
-      <c r="C353" s="12"/>
+      <c r="C353" s="9"/>
       <c r="D353" s="1"/>
       <c r="E353" s="1"/>
       <c r="F353" s="1"/>
@@ -5791,7 +5803,7 @@
     <row r="354" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="1"/>
       <c r="B354" s="1"/>
-      <c r="C354" s="12"/>
+      <c r="C354" s="9"/>
       <c r="D354" s="1"/>
       <c r="E354" s="1"/>
       <c r="F354" s="1"/>
@@ -5803,7 +5815,7 @@
     <row r="355" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A355" s="1"/>
       <c r="B355" s="1"/>
-      <c r="C355" s="12"/>
+      <c r="C355" s="9"/>
       <c r="D355" s="1"/>
       <c r="E355" s="1"/>
       <c r="F355" s="1"/>

</xml_diff>

<commit_message>
method refererence+ fucntional demos
</commit_message>
<xml_diff>
--- a/globallogic_mcqtest.xlsx
+++ b/globallogic_mcqtest.xlsx
@@ -853,11 +853,11 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C160" activeCellId="0" sqref="C160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C146" activeCellId="0" sqref="C146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="22.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="22.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.57"/>

</xml_diff>